<commit_message>
have added the functionality to convert the months into dhis2 format
</commit_message>
<xml_diff>
--- a/master_facilities.xlsx
+++ b/master_facilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blessings/Desktop/compare-dvdmt-facilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16E05AA-D19E-5848-9E17-0D78EAC0FB34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66516E14-9603-8B4C-8CC6-7BC16EF84B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33060" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3056" uniqueCount="1439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3100" uniqueCount="1453">
   <si>
     <t>Central East</t>
   </si>
@@ -4347,17 +4347,83 @@
   </si>
   <si>
     <t>dhis2_name</t>
+  </si>
+  <si>
+    <t>Machinga HC</t>
+  </si>
+  <si>
+    <t>Monkey Bay</t>
+  </si>
+  <si>
+    <t>St Martins</t>
+  </si>
+  <si>
+    <t>Mtimabi</t>
+  </si>
+  <si>
+    <t>Mangochi Hosp</t>
+  </si>
+  <si>
+    <t>Mulibwanji</t>
+  </si>
+  <si>
+    <t>katema</t>
+  </si>
+  <si>
+    <t>CHIRINGA CHAM</t>
+  </si>
+  <si>
+    <t>Chiringa Maternity</t>
+  </si>
+  <si>
+    <t>Namikango Maternity</t>
+  </si>
+  <si>
+    <t>Namikango Health Centre</t>
+  </si>
+  <si>
+    <t>Lungadzi Outreach Clinic</t>
+  </si>
+  <si>
+    <t>Elaine Zakresk PVT</t>
+  </si>
+  <si>
+    <t>Elaine Zakresh Outreach Clinic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4380,8 +4446,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4699,10 +4769,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D764"/>
+  <dimension ref="A1:D775"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E841" sqref="E841"/>
+    <sheetView tabSelected="1" topLeftCell="A735" workbookViewId="0">
+      <selection activeCell="J777" sqref="J777"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15403,6 +15473,160 @@
         <v>1434</v>
       </c>
     </row>
+    <row r="765" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A765" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B765" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C765" s="2" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D765" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="766" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A766" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B766" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C766" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D766" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="767" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A767" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B767" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C767" s="2" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D767" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="768" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A768" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B768" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C768" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D768" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="769" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A769" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B769" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C769" s="2" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D769" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="770" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A770" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B770" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C770" s="2" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D770" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="771" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A771" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B771" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C771" s="2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D771" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="772" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A772" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B772" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C772" s="2" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D772" s="3" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="773" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B773" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C773" s="2" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D773" s="3" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="774" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A774" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B774" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C774" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D774" s="4" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="775" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B775" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C775" s="2" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D775" s="3" t="s">
+        <v>1452</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>